<commit_message>
fix ~$ enumerator list
</commit_message>
<xml_diff>
--- a/FishLandings/data/enumerator_list.xlsx
+++ b/FishLandings/data/enumerator_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86753B54-8E0D-7043-810E-44E250D87D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E8A9A-B0BD-8B49-B913-F1D49D6D986E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21080" yWindow="3920" windowWidth="10000" windowHeight="12660" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
QC and CUE, relative abundance scripts
</commit_message>
<xml_diff>
--- a/FishLandings/data/enumerator_list.xlsx
+++ b/FishLandings/data/enumerator_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E8A9A-B0BD-8B49-B913-F1D49D6D986E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5ADBFC-57AB-2640-83A1-75C7879A1F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21080" yWindow="3920" windowWidth="10000" windowHeight="12660" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
+    <workbookView xWindow="11180" yWindow="8080" windowWidth="19900" windowHeight="10540" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>BMU</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>landing_site</t>
+  </si>
+  <si>
+    <t>Ngala</t>
+  </si>
+  <si>
+    <t>Edward Yaa</t>
   </si>
 </sst>
 </file>
@@ -506,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27ABF6E-FCDE-A64A-8E31-FB070AB67392}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,10 +804,10 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,10 +815,10 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -820,9 +826,31 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>